<commit_message>
modified pcb components bom
</commit_message>
<xml_diff>
--- a/hardware/BOM/PCB components.xlsx
+++ b/hardware/BOM/PCB components.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="355">
   <si>
     <t>Component</t>
   </si>
@@ -97,21 +97,12 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Re1</t>
-  </si>
-  <si>
     <t>valve connector</t>
   </si>
   <si>
-    <t>Re2</t>
-  </si>
-  <si>
     <t>pump connector</t>
   </si>
   <si>
-    <t>Re3</t>
-  </si>
-  <si>
     <t>convert 12V to 5V to power 5V components. Package type TO-263 i.e. LM2596HVT -5.0 or LM2596T -5.0 [the one used in simulation has a rating of 1A. Change this to 3A when sourcing]</t>
   </si>
   <si>
@@ -193,9 +184,6 @@
     <t>schottky Diode</t>
   </si>
   <si>
-    <t>resitor</t>
-  </si>
-  <si>
     <t>5.1 k</t>
   </si>
   <si>
@@ -292,27 +280,6 @@
     <t>R8</t>
   </si>
   <si>
-    <t>conn_1</t>
-  </si>
-  <si>
-    <t>reg</t>
-  </si>
-  <si>
-    <t>conv</t>
-  </si>
-  <si>
-    <t>usb</t>
-  </si>
-  <si>
-    <t>led_1</t>
-  </si>
-  <si>
-    <t>SW_1</t>
-  </si>
-  <si>
-    <t>SW_2</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -322,15 +289,6 @@
     <t>Q3</t>
   </si>
   <si>
-    <t>conn_2</t>
-  </si>
-  <si>
-    <t>conn_3</t>
-  </si>
-  <si>
-    <t>conn_4</t>
-  </si>
-  <si>
     <t>Input 12V from the battery consider a two pin connector Screw Terminal Block (2-pin, 5.08mm pitch)</t>
   </si>
   <si>
@@ -983,6 +941,153 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>D10</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1499,7 +1604,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
@@ -1508,16 +1613,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>4</v>
@@ -1549,38 +1654,38 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>334</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="J3" s="2">
         <v>0.91</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
@@ -1591,76 +1696,76 @@
         <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="J4" s="2">
         <v>0.4</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2">
         <v>1.34</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
@@ -1672,34 +1777,34 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="J6" s="2">
         <v>0.44</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1707,43 +1812,43 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="J8" s="4">
         <v>0.64</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
@@ -1752,31 +1857,31 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="J9" s="4">
         <v>0.49</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="M9" s="23"/>
     </row>
@@ -1789,31 +1894,31 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="J10" s="4">
         <v>0.44</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="M10" s="23"/>
     </row>
@@ -1825,73 +1930,73 @@
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="J11" s="4">
         <v>0.88</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="M11" s="23"/>
     </row>
     <row r="12" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="J12" s="4">
         <v>0.55000000000000004</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="M12" s="23"/>
     </row>
@@ -1900,261 +2005,269 @@
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>90</v>
+        <v>306</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="J14" s="7">
         <v>0.51</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
         <v>0.59</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7">
         <v>0.59</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="M16" s="25"/>
     </row>
     <row r="19" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="C19" s="27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10">
         <v>0.1</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M19" s="28"/>
     </row>
     <row r="20" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="C20" s="27"/>
       <c r="D20" s="10" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="J20" s="10">
         <v>0.04</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="M20" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="C21" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10">
         <v>0.1</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M21" s="28"/>
     </row>
     <row r="22" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="B22" s="10"/>
+        <v>226</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="J22" s="10">
         <v>1.36</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="M22" s="28" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="J25" s="9">
         <f>SUM(J3:J22)</f>
@@ -2171,9 +2284,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2205,7 +2318,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
@@ -2214,16 +2327,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>4</v>
@@ -2252,38 +2365,38 @@
     </row>
     <row r="3" spans="1:13" s="33" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>149</v>
+        <v>331</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="J3" s="31">
         <v>5.61</v>
       </c>
       <c r="K3" s="31" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="M3" s="32"/>
     </row>
@@ -2295,499 +2408,499 @@
     </row>
     <row r="5" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="J5" s="4">
         <v>0.42</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4">
         <v>0.64</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>92</v>
+        <v>335</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="J9" s="7">
         <v>0.89</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="J10" s="7">
         <v>0.44</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7">
         <v>0.1</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M11" s="25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7">
         <v>0.1</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="29" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>94</v>
+        <v>332</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="J15" s="10">
         <v>0.53</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:13" s="29" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10">
         <v>0.1</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M16" s="28"/>
     </row>
     <row r="17" spans="1:13" s="29" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10">
         <v>0.59</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="M17" s="28"/>
     </row>
     <row r="18" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>95</v>
+        <v>333</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="J20" s="11">
         <v>0.53</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="M20" s="35"/>
     </row>
     <row r="21" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11">
         <v>0.1</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M21" s="35"/>
     </row>
     <row r="23" spans="1:13" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="37" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="J23" s="38">
         <v>0.1</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="L23" s="38" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="M23" s="39"/>
     </row>
     <row r="24" spans="1:13" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I24" s="38"/>
       <c r="J24" s="38">
         <v>0.1</v>
       </c>
       <c r="K24" s="38" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L24" s="38" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M24" s="39"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="J28" s="9">
         <f>SUM(J3:J24)</f>
@@ -2806,13 +2919,13 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.36328125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8" style="9" customWidth="1"/>
     <col min="3" max="3" width="7.90625" style="9" customWidth="1"/>
     <col min="4" max="4" width="13.7265625" style="9" customWidth="1"/>
     <col min="5" max="5" width="13.6328125" style="9" customWidth="1"/>
@@ -2838,7 +2951,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
@@ -2847,16 +2960,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>4</v>
@@ -2877,304 +2990,304 @@
     </row>
     <row r="3" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>24</v>
+        <v>351</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="2" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="J3" s="2">
         <v>1.51</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2">
         <v>0.05</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="2" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="J5" s="2">
         <v>0.04</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2">
         <v>0.1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="J7" s="2">
         <v>0.55000000000000004</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="M7" s="21"/>
     </row>
     <row r="8" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2">
         <v>0.05</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="M8" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2">
         <v>0.64</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="M9" s="21"/>
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>99</v>
+        <v>336</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="J10" s="2">
         <v>0.91</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -3184,611 +3297,611 @@
     </row>
     <row r="12" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>26</v>
+        <v>352</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="4" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="J12" s="4">
         <v>1.51</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="4" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4">
         <v>0.05</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="M13" s="23"/>
     </row>
     <row r="14" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>97</v>
+        <v>329</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="4" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="J14" s="4">
         <v>0.04</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>87</v>
+        <v>312</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4">
         <v>0.1</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M15" s="23"/>
     </row>
     <row r="16" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="J16" s="4">
         <v>0.55000000000000004</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="M16" s="23"/>
     </row>
     <row r="17" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="4" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4">
         <v>0.05</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="M17" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4">
         <v>0.64</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="M18" s="23"/>
     </row>
     <row r="19" spans="1:13" s="24" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>100</v>
+        <v>337</v>
       </c>
       <c r="C19" s="42"/>
       <c r="D19" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="J19" s="4">
         <v>0.91</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M19" s="23" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>28</v>
+        <v>353</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="7" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="J22" s="7">
         <v>1.51</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="7" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7">
         <v>0.05</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>98</v>
+        <v>330</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="7" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="J24" s="7">
         <v>0.04</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="M24" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>88</v>
+        <v>313</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7">
         <v>0.1</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="J26" s="7">
         <v>0.55000000000000004</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>86</v>
+        <v>354</v>
       </c>
       <c r="C27" s="34"/>
       <c r="D27" s="7" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7">
         <v>0.05</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="M27" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7">
         <v>0.64</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" s="26" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>101</v>
+        <v>338</v>
       </c>
       <c r="C29" s="34"/>
       <c r="D29" s="7" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="J29" s="7">
         <v>0.91</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="M29" s="25" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="J33" s="9">
         <f>SUM(J3:J30)</f>
@@ -3806,14 +3919,14 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="5.08984375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" style="9" customWidth="1"/>
     <col min="3" max="3" width="7.90625" style="9" customWidth="1"/>
     <col min="4" max="5" width="13.7265625" style="9" customWidth="1"/>
     <col min="6" max="7" width="12.6328125" style="9" customWidth="1"/>
@@ -3835,7 +3948,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
@@ -3844,16 +3957,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>4</v>
@@ -3873,852 +3986,898 @@
     </row>
     <row r="3" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>339</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J3" s="2">
         <v>0.2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>314</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2">
         <v>0.1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>315</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2">
         <v>0.1</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>236</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2">
         <v>0.64</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>246</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>340</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J8" s="4">
         <v>0.2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>316</v>
+      </c>
       <c r="C9" s="43" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4">
         <v>0.1</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M9" s="23"/>
     </row>
     <row r="10" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>317</v>
+      </c>
       <c r="C10" s="4" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4">
         <v>0.1</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M10" s="23"/>
     </row>
     <row r="11" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>236</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>308</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4">
         <v>0.64</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="B13" s="7"/>
+        <v>247</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>341</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J13" s="7">
         <v>0.2</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="M13" s="25" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="C14" s="44" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7">
         <v>0.1</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="C15" s="7" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
         <v>0.1</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:14" s="29" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="B17" s="10"/>
+        <v>248</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>342</v>
+      </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="G17" s="45" t="s">
-        <v>265</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>267</v>
       </c>
       <c r="J17" s="10">
         <v>0.4</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="M17" s="28" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="B19" s="11"/>
+        <v>247</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>343</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="J19" s="11">
         <v>0.2</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>320</v>
+      </c>
       <c r="C20" s="46" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11">
         <v>0.1</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M20" s="35"/>
     </row>
     <row r="21" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>321</v>
+      </c>
       <c r="C21" s="11" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11">
         <v>0.1</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M21" s="35"/>
     </row>
     <row r="23" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="B23" s="38"/>
+        <v>234</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>344</v>
+      </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J23" s="38">
         <v>0.2</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L23" s="38" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="M23" s="39" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="38"/>
+        <v>43</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>322</v>
+      </c>
       <c r="C24" s="47" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I24" s="38"/>
       <c r="J24" s="38">
         <v>0.1</v>
       </c>
       <c r="K24" s="38" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L24" s="38" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M24" s="39"/>
     </row>
     <row r="25" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="B25" s="38"/>
+        <v>236</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>309</v>
+      </c>
       <c r="C25" s="38" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I25" s="38" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="J25" s="38"/>
       <c r="K25" s="38">
         <v>0.64</v>
       </c>
       <c r="L25" s="38" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="M25" s="39" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="N25" s="40" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="48" t="s">
-        <v>274</v>
-      </c>
-      <c r="B27" s="49"/>
+        <v>260</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>345</v>
+      </c>
       <c r="C27" s="49"/>
       <c r="D27" s="49" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F27" s="49" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G27" s="49" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="H27" s="49" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I27" s="49" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J27" s="49">
         <v>0.2</v>
       </c>
       <c r="K27" s="49" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L27" s="49" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="49"/>
+        <v>43</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>323</v>
+      </c>
       <c r="C28" s="52" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="E28" s="53" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F28" s="49" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G28" s="49" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H28" s="49" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I28" s="49"/>
       <c r="J28" s="49">
         <v>0.1</v>
       </c>
       <c r="K28" s="49" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L28" s="49" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M28" s="50"/>
     </row>
     <row r="29" spans="1:14" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="48" t="s">
-        <v>250</v>
-      </c>
-      <c r="B29" s="49"/>
+        <v>236</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>310</v>
+      </c>
       <c r="C29" s="49" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E29" s="49" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F29" s="49" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="H29" s="49" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="J29" s="49"/>
       <c r="K29" s="49">
         <v>0.64</v>
       </c>
       <c r="L29" s="49" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="N29" s="51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="54" t="s">
-        <v>275</v>
-      </c>
-      <c r="B32" s="55"/>
+        <v>261</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>346</v>
+      </c>
       <c r="C32" s="55"/>
       <c r="D32" s="55" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="F32" s="55" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="G32" s="55" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="I32" s="55" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="J32" s="55">
         <v>0.03</v>
       </c>
       <c r="K32" s="55" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="L32" s="55" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="M32" s="56"/>
     </row>
     <row r="33" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="54" t="s">
-        <v>276</v>
-      </c>
-      <c r="B33" s="55"/>
+        <v>262</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>324</v>
+      </c>
       <c r="C33" s="55" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D33" s="55" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="F33" s="55" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="G33" s="55" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="H33" s="55" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="I33" s="55" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="J33" s="55">
         <v>0.3</v>
       </c>
       <c r="K33" s="55" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="L33" s="55" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="M33" s="56" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="J37" s="9">
         <f>SUM(J3:J35)</f>
@@ -4735,13 +4894,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" style="12" customWidth="1"/>
     <col min="2" max="3" width="8.7265625" style="9"/>
     <col min="4" max="4" width="11.7265625" style="9" customWidth="1"/>
     <col min="5" max="5" width="14.36328125" style="9" customWidth="1"/>
@@ -4763,7 +4922,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
@@ -4772,16 +4931,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>4</v>
@@ -4795,252 +4954,264 @@
     </row>
     <row r="3" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>281</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>347</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="J3" s="2">
         <v>0.31</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="M3" s="21"/>
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>325</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2">
         <v>0.1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="C5" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2">
         <v>0.1</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>311</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2">
         <v>0.64</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>288</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="J9" s="4">
         <v>0.48</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="M9" s="23"/>
     </row>
     <row r="12" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="B12" s="7"/>
+        <v>304</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>349</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="J12" s="7">
         <v>0.31</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>82</v>
+        <v>327</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7">
         <v>0.1</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M13" s="25"/>
     </row>
@@ -5052,79 +5223,81 @@
     </row>
     <row r="16" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="B16" s="10"/>
+        <v>303</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>350</v>
+      </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="J16" s="10">
         <v>0.31</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="M16" s="28"/>
     </row>
     <row r="17" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>82</v>
+        <v>328</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10">
         <v>0.1</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="M17" s="28"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="J21" s="9">
         <f>SUM(J3:J17)</f>

</xml_diff>

<commit_message>
finalized the power management schematic
</commit_message>
<xml_diff>
--- a/hardware/BOM/PCB components.xlsx
+++ b/hardware/BOM/PCB components.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="356">
   <si>
     <t>Component</t>
   </si>
@@ -1088,6 +1088,9 @@
   </si>
   <si>
     <t>D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L </t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1576,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1584,7 +1587,7 @@
     <col min="4" max="4" width="12.7265625" style="9" customWidth="1"/>
     <col min="5" max="5" width="13.453125" style="9" customWidth="1"/>
     <col min="6" max="6" width="13.08984375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" style="9" customWidth="1"/>
     <col min="8" max="9" width="9.90625" style="9" customWidth="1"/>
     <col min="10" max="10" width="8.7265625" style="9"/>
     <col min="11" max="11" width="10.36328125" style="9" customWidth="1"/>
@@ -1942,7 +1945,7 @@
         <v>175</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>175</v>
+        <v>355</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>179</v>
@@ -3919,8 +3922,8 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>